<commit_message>
added results and made update_evasive_list use exact sample names
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Datum</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>14.12.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbesserung des Prototypen (Rewriter funktioniert, Minimizer und Cleanup noch nicht)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update der Dokumentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testen des Prototypen</t>
   </si>
   <si>
     <t>total</t>
@@ -1319,34 +1328,44 @@
       </c>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B46">
         <v>6</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" ht="14.25">
       <c r="A48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="49" ht="14.25">
       <c r="A49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="50" ht="14.25">
       <c r="A50" s="2"/>
@@ -1358,11 +1377,11 @@
     </row>
     <row r="52" ht="14.25">
       <c r="A52" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B52" s="5">
         <f>SUM(B2:B51)</f>
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in update_working_list
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Datum</t>
   </si>
@@ -204,10 +204,10 @@
     <t xml:space="preserve">Verbesserung des Prototypen (Triage der initialen samples zwischen av und ml-modell)</t>
   </si>
   <si>
-    <t>13.12.2024</t>
-  </si>
-  <si>
-    <t>14.12.2024</t>
+    <t>23.12.2024</t>
+  </si>
+  <si>
+    <t>24.12.2024</t>
   </si>
   <si>
     <t xml:space="preserve">Verbesserung des Prototypen (Rewriter funktioniert, Minimizer und Cleanup noch nicht)</t>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t xml:space="preserve">Testen des Prototypen</t>
+  </si>
+  <si>
+    <t>25.12.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbesserung, Testen und Debuggen des Prototypen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vergleich des aktuellen Prototypen mit dem Original</t>
   </si>
   <si>
     <t>total</t>
@@ -862,7 +871,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1328,24 +1337,24 @@
       </c>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B46">
         <v>6</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B47">
         <v>6</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1354,7 +1363,7 @@
       <c r="B48">
         <v>1</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1363,25 +1372,37 @@
       <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" ht="14.25">
-      <c r="A50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="A50" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="51" ht="14.25">
       <c r="A51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="52" ht="14.25">
       <c r="A52" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B52" s="5">
         <f>SUM(B2:B51)</f>
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added evaluation script results
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Datum</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dokumentation und Testen des Prototypen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schreiben von Evaluierungsscript und starten der Evaluierung</t>
   </si>
   <si>
     <t>total</t>
@@ -1334,7 +1337,7 @@
       </c>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B46">
@@ -1345,13 +1348,13 @@
       </c>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B47">
         <v>6</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1360,7 +1363,7 @@
       <c r="B48">
         <v>1</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1369,32 +1372,37 @@
       <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" ht="14.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B50">
         <v>6</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="51" ht="14.25">
       <c r="A51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="52" ht="14.25">
       <c r="A52" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B52" s="5">
         <f>SUM(B2:B51)</f>
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added concept part to documentation
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Datum</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kommentieren von Code, Schreiben von Dokumentation und Code Hygiene</t>
+  </si>
+  <si>
+    <t>30.12.2024</t>
   </si>
   <si>
     <t>total</t>
@@ -1443,19 +1446,23 @@
       </c>
     </row>
     <row r="54" ht="14.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="2">
         <v>10</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="55" ht="14.25">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
+      <c r="A55" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="2">
+        <v>9</v>
+      </c>
       <c r="C55" s="2"/>
     </row>
     <row r="56" ht="14.25">
@@ -1495,11 +1502,11 @@
     </row>
     <row r="63" ht="14.25">
       <c r="A63" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B63" s="5">
         <f>SUM(B2:B62)</f>
-        <v>233</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added debug and eval results for ember
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -910,7 +910,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A48" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1498,7 +1498,7 @@
         <v>81</v>
       </c>
       <c r="B57" s="2">
-        <v>5.5</v>
+        <v>7.5</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>82</v>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="B63" s="5">
         <f>SUM(B2:B62)</f>
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed Dockerfile back to old one
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Datum</t>
   </si>
@@ -265,6 +265,21 @@
   </si>
   <si>
     <t xml:space="preserve">Bauen eines eigenständigen Docker Images (mit GPU support)</t>
+  </si>
+  <si>
+    <t>03.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Docker troubleshooting (lief ember mismatch)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ember neu trainieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Troubleshooting Lief</t>
+  </si>
+  <si>
+    <t>04.01.2025</t>
   </si>
   <si>
     <t>total</t>
@@ -910,7 +925,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1483,45 +1498,63 @@
       </c>
     </row>
     <row r="56" ht="14.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B56" s="2">
         <v>5</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="57" ht="14.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B57" s="2">
         <v>7.5</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="58" ht="14.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="A58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="2">
+        <v>4</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="59" ht="14.25">
       <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="B59" s="2">
+        <v>4</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="60" ht="14.25">
       <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="B60" s="2">
+        <v>2</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="61" ht="14.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
+      <c r="A61" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" s="2">
+        <v>3</v>
+      </c>
       <c r="C61" s="2"/>
     </row>
     <row r="62" ht="14.25">
@@ -1530,12 +1563,15 @@
       <c r="C62" s="2"/>
     </row>
     <row r="63" ht="14.25">
-      <c r="A63" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B63" s="5">
-        <f>SUM(B2:B62)</f>
-        <v>267</v>
+      <c r="B63"/>
+    </row>
+    <row r="72" ht="14.25">
+      <c r="A72" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B72" s="5">
+        <f>SUM(B2:B71)</f>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Meeting notes, TODOs and Documentation
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Datum</t>
   </si>
@@ -280,6 +280,30 @@
   </si>
   <si>
     <t>04.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pytorch GPU troubleshooting</t>
+  </si>
+  <si>
+    <t>05.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluierung MAB-malware av modus</t>
+  </si>
+  <si>
+    <t>06.01.2025</t>
+  </si>
+  <si>
+    <t>07.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debuggen des MAB-malware av modus</t>
+  </si>
+  <si>
+    <t>08.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pytorch Container test</t>
   </si>
   <si>
     <t>total</t>
@@ -925,7 +949,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1549,29 +1573,75 @@
       </c>
     </row>
     <row r="61" ht="14.25">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B61" s="2">
         <v>3</v>
       </c>
-      <c r="C61" s="2"/>
+      <c r="C61" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="62" ht="14.25">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="A62" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="2">
+        <v>2</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="63" ht="14.25">
-      <c r="B63"/>
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" ht="14.25">
+      <c r="A64" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" ht="14.25">
+      <c r="A65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" ht="14.25">
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="5" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B72" s="5">
         <f>SUM(B2:B71)</f>
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Zeitaufzeichnung that was broken by merge
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Datum</t>
   </si>
@@ -280,6 +280,39 @@
   </si>
   <si>
     <t>04.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evalusierung AV modus</t>
+  </si>
+  <si>
+    <t>05.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Troubleshooting AV modus</t>
+  </si>
+  <si>
+    <t>06.01.2025</t>
+  </si>
+  <si>
+    <t>07.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluierung av modus</t>
+  </si>
+  <si>
+    <t>08.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluierung AV modus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pytorch troubleshooting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vorbereitung für Meeting</t>
+  </si>
+  <si>
+    <t>09.01.2025</t>
   </si>
   <si>
     <t>total</t>
@@ -925,7 +958,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1549,29 +1582,94 @@
       </c>
     </row>
     <row r="61" ht="14.25">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B61" s="2">
         <v>3</v>
       </c>
-      <c r="C61" s="2"/>
+      <c r="C61" s="4" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="62" ht="14.25">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="A62" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="2">
+        <v>4</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="63" ht="14.25">
-      <c r="B63"/>
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" ht="14.25">
+      <c r="A64" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" ht="14.25">
+      <c r="A65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" ht="14.25">
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" ht="14.25">
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" ht="14.25">
+      <c r="A68" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="5" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B72" s="5">
         <f>SUM(B2:B71)</f>
-        <v>280</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed gitignore and time booking
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Datum</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t xml:space="preserve">Fertigstellung Dockerimage mit GPU support</t>
+  </si>
+  <si>
+    <t>11.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check der Samples auf Funktionalität</t>
+  </si>
+  <si>
+    <t>12.01.2025</t>
   </si>
   <si>
     <t>total</t>
@@ -960,7 +969,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A51" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1673,13 +1682,36 @@
         <v>99</v>
       </c>
     </row>
-    <row r="72" ht="14.25">
-      <c r="A72" s="4" t="s">
+    <row r="70" ht="14.25">
+      <c r="A70" t="s">
         <v>100</v>
       </c>
-      <c r="B72" s="4">
-        <f>SUM(B2:B71)</f>
-        <v>294</v>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" ht="14.25">
+      <c r="A71" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="72" ht="14.25"/>
+    <row r="96" ht="14.25">
+      <c r="A96" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B96" s="4">
+        <f>SUM(B2:B95)</f>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
analysis of 20 random samples
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Datum</t>
   </si>
@@ -321,10 +321,16 @@
     <t>11.01.2025</t>
   </si>
   <si>
-    <t xml:space="preserve">Check der Samples auf Funktionalität</t>
+    <t xml:space="preserve">Check der Samples auf Funktionalität (Generieren von Samples)</t>
   </si>
   <si>
     <t>12.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check der Samples auf Funktionalität (Generieren von Samples und Auswahl der Stichproben)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamische Analyse der Modifizierten Malware Samples</t>
   </si>
   <si>
     <t>total</t>
@@ -969,7 +975,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A63" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1701,17 +1707,24 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="72" ht="14.25"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" ht="14.25">
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="C72" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="96" ht="14.25">
       <c r="A96" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B96" s="4">
         <f>SUM(B2:B95)</f>
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Timetracking in advance in case I break everything
</commit_message>
<xml_diff>
--- a/Documentation/Zeitaufzeichnung.xlsx
+++ b/Documentation/Zeitaufzeichnung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Datum</t>
   </si>
@@ -352,6 +352,33 @@
   </si>
   <si>
     <t xml:space="preserve">Bauen eines eigenständigen Docker Images &amp; anpassen der Dokumentation</t>
+  </si>
+  <si>
+    <t>27.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anpassen der Dokumentation</t>
+  </si>
+  <si>
+    <t>28.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code optimierung</t>
+  </si>
+  <si>
+    <t>29.01.2025</t>
+  </si>
+  <si>
+    <t>30.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleanup des git repos und Tests</t>
+  </si>
+  <si>
+    <t>31.01.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tests und Abgabe des Projekts</t>
   </si>
   <si>
     <t>total</t>
@@ -996,7 +1023,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A72" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1794,13 +1821,68 @@
         <v>111</v>
       </c>
     </row>
+    <row r="78" ht="14.25">
+      <c r="A78" t="s">
+        <v>112</v>
+      </c>
+      <c r="B78">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="79" ht="14.25">
+      <c r="A79" t="s">
+        <v>114</v>
+      </c>
+      <c r="B79">
+        <v>6</v>
+      </c>
+      <c r="C79" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" ht="14.25">
+      <c r="A80" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" ht="14.25">
+      <c r="A81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="82" ht="14.25">
+      <c r="A82" t="s">
+        <v>119</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="96" ht="14.25">
       <c r="A96" s="4" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B96" s="4">
         <f>SUM(B2:B95)</f>
-        <v>332</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>